<commit_message>
results table of mixed model 1 (mm1)
</commit_message>
<xml_diff>
--- a/mm1_results.xlsx
+++ b/mm1_results.xlsx
@@ -84,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +98,26 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="5"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,11 +132,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -132,6 +142,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -413,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -424,18 +440,18 @@
     <col min="1" max="1" width="20.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -445,198 +461,199 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>0.122</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.128</v>
-      </c>
-      <c r="D2" s="4">
-        <v>-0.14430158000000001</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.38510328999999999</v>
-      </c>
-      <c r="F2" s="4"/>
+      <c r="C2" s="3">
+        <v>0.12814</v>
+      </c>
+      <c r="D2" s="3">
+        <v>-0.13400000000000001</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.372</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="D3" s="4">
-        <v>4.2905489999999998E-2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.55870251000000004</v>
-      </c>
-      <c r="F3" s="4">
-        <v>5.1230000000000002</v>
+      <c r="B3" s="3">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.13217000000000001</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F3" s="3">
+        <v>5.1070000000000002</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="4">
-        <v>2.3609999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H3" s="1">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="D4" s="4">
-        <v>-0.20817985999999999</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.34094423000000001</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.19570000000000001</v>
+      <c r="B4" s="3">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.13299</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-0.216</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.185</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="4">
-        <v>0.65822000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H4" s="1">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1">
-        <v>-9.1999999999999998E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>-0.23132593000000001</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3.225894E-2</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.9829000000000001</v>
+      <c r="B5" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6.5839999999999996E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-0.22700000000000001</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2.3220000000000001</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="4">
-        <v>0.15909000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H5" s="1">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1">
-        <v>-0.10299999999999999</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="D6" s="4">
-        <v>-0.38250426999999998</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.16688394000000001</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.56340000000000001</v>
+      <c r="B6" s="3">
+        <v>-8.4000000000000005E-2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.13749</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-0.36099999999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.184</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.371</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="4">
-        <v>0.45289000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H6" s="1">
+        <v>0.54300000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
-        <v>-6.0000000000000001E-3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="D7" s="4">
-        <v>-0.13692947999999999</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.14212303000000001</v>
-      </c>
-      <c r="F7" s="4">
-        <v>6.8999999999999999E-3</v>
+      <c r="B7" s="3">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6.7369999999999999E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.121</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="4">
-        <v>0.93393000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H7" s="1">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="D8" s="4">
-        <v>-3.1291760000000002E-2</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.22683587999999999</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1.8925000000000001</v>
+      <c r="B8" s="3">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>6.7409999999999998E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.9570000000000001</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="4">
-        <v>0.16891999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H8" s="1">
+        <v>0.16200000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>

</xml_diff>